<commit_message>
Data analysis in excel
</commit_message>
<xml_diff>
--- a/Sorted Data for visualisation.xlsx
+++ b/Sorted Data for visualisation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Character mentions" sheetId="1" r:id="rId1"/>
@@ -1009,7 +1009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -1331,7 +1331,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A15"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1475,7 +1475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Web version of visualisation
</commit_message>
<xml_diff>
--- a/Sorted Data for visualisation.xlsx
+++ b/Sorted Data for visualisation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Character mentions" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="55">
   <si>
     <t>Alice_count</t>
   </si>
@@ -175,12 +175,27 @@
   </si>
   <si>
     <t>Sister</t>
+  </si>
+  <si>
+    <t>pun p</t>
+  </si>
+  <si>
+    <t>rhyme p</t>
+  </si>
+  <si>
+    <t>logic p</t>
+  </si>
+  <si>
+    <t>size p</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.0"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -288,8 +303,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="63">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1007,19 +1023,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:11">
       <c r="B1" t="s">
         <v>25</v>
       </c>
@@ -1030,16 +1048,28 @@
         <v>27</v>
       </c>
       <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" t="s">
         <v>29</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="K1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1052,17 +1082,33 @@
       <c r="D2">
         <v>2</v>
       </c>
-      <c r="E2">
-        <v>0</v>
+      <c r="E2" s="1">
+        <f>D2/39%</f>
+        <v>5.1282051282051277</v>
       </c>
       <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <f>F2/41%</f>
+        <v>0</v>
+      </c>
+      <c r="H2">
         <v>1</v>
       </c>
-      <c r="G2">
+      <c r="I2" s="1">
+        <f>H2/31%</f>
+        <v>3.2258064516129035</v>
+      </c>
+      <c r="J2">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="K2" s="1">
+        <f>J2/24%</f>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1075,17 +1121,33 @@
       <c r="D3">
         <v>2</v>
       </c>
-      <c r="E3">
-        <v>2</v>
+      <c r="E3" s="1">
+        <f t="shared" ref="E3:E13" si="0">D3/39%</f>
+        <v>5.1282051282051277</v>
       </c>
       <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1">
+        <f t="shared" ref="G3:G13" si="1">F3/41%</f>
+        <v>4.8780487804878048</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" ref="I3:I13" si="2">H3/31%</f>
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3" s="1">
+        <f t="shared" ref="K3:K13" si="3">J3/24%</f>
+        <v>8.3333333333333339</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1098,17 +1160,33 @@
       <c r="D4">
         <v>4</v>
       </c>
-      <c r="E4">
-        <v>0</v>
+      <c r="E4" s="1">
+        <f t="shared" si="0"/>
+        <v>10.256410256410255</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="K4" s="1">
+        <f t="shared" si="3"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1121,17 +1199,33 @@
       <c r="D5">
         <v>0</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H5">
         <v>3</v>
       </c>
-      <c r="G5">
+      <c r="I5" s="1">
+        <f t="shared" si="2"/>
+        <v>9.67741935483871</v>
+      </c>
+      <c r="J5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="K5" s="1">
+        <f t="shared" si="3"/>
+        <v>16.666666666666668</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1144,17 +1238,33 @@
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
+        <v>2.5641025641025639</v>
+      </c>
+      <c r="F6">
         <v>6</v>
       </c>
-      <c r="F6">
-        <v>2</v>
-      </c>
-      <c r="G6">
+      <c r="G6" s="1">
+        <f t="shared" si="1"/>
+        <v>14.634146341463415</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="2"/>
+        <v>6.4516129032258069</v>
+      </c>
+      <c r="J6">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="K6" s="1">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1167,17 +1277,33 @@
       <c r="D7">
         <v>2</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
+        <f t="shared" si="0"/>
+        <v>5.1282051282051277</v>
+      </c>
+      <c r="F7">
         <v>4</v>
       </c>
-      <c r="F7">
+      <c r="G7" s="1">
+        <f t="shared" si="1"/>
+        <v>9.7560975609756095</v>
+      </c>
+      <c r="H7">
         <v>1</v>
       </c>
-      <c r="G7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="I7" s="1">
+        <f t="shared" si="2"/>
+        <v>3.2258064516129035</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7" s="1">
+        <f t="shared" si="3"/>
+        <v>8.3333333333333339</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1190,17 +1316,33 @@
       <c r="D8">
         <v>5</v>
       </c>
-      <c r="E8">
-        <v>2</v>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>12.820512820512819</v>
       </c>
       <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="1"/>
+        <v>4.8780487804878048</v>
+      </c>
+      <c r="H8">
         <v>3</v>
       </c>
-      <c r="G8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="I8" s="1">
+        <f t="shared" si="2"/>
+        <v>9.67741935483871</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8" s="1">
+        <f t="shared" si="3"/>
+        <v>8.3333333333333339</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1213,17 +1355,33 @@
       <c r="D9">
         <v>0</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H9">
         <v>4</v>
       </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="I9" s="1">
+        <f t="shared" si="2"/>
+        <v>12.903225806451614</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1236,17 +1394,33 @@
       <c r="D10">
         <v>13</v>
       </c>
-      <c r="E10">
-        <v>0</v>
+      <c r="E10" s="1">
+        <f t="shared" si="0"/>
+        <v>33.333333333333336</v>
       </c>
       <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H10">
         <v>9</v>
       </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="I10" s="1">
+        <f t="shared" si="2"/>
+        <v>29.032258064516128</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1259,17 +1433,33 @@
       <c r="D11">
         <v>4</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
+        <f t="shared" si="0"/>
+        <v>10.256410256410255</v>
+      </c>
+      <c r="F11">
         <v>18</v>
       </c>
-      <c r="F11">
+      <c r="G11" s="1">
+        <f t="shared" si="1"/>
+        <v>43.902439024390247</v>
+      </c>
+      <c r="H11">
         <v>4</v>
       </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="I11" s="1">
+        <f t="shared" si="2"/>
+        <v>12.903225806451614</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1282,17 +1472,33 @@
       <c r="D12">
         <v>4</v>
       </c>
-      <c r="E12">
-        <v>2</v>
+      <c r="E12" s="1">
+        <f t="shared" si="0"/>
+        <v>10.256410256410255</v>
       </c>
       <c r="F12">
         <v>2</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="1">
+        <f t="shared" si="1"/>
+        <v>4.8780487804878048</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="2"/>
+        <v>6.4516129032258069</v>
+      </c>
+      <c r="J12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="K12" s="1">
+        <f t="shared" si="3"/>
+        <v>4.166666666666667</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1305,14 +1511,48 @@
       <c r="D13">
         <v>2</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
+        <f t="shared" si="0"/>
+        <v>5.1282051282051277</v>
+      </c>
+      <c r="F13">
         <v>7</v>
       </c>
-      <c r="F13">
-        <v>2</v>
-      </c>
-      <c r="G13">
+      <c r="G13" s="1">
+        <f t="shared" si="1"/>
+        <v>17.073170731707318</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="2"/>
+        <v>6.4516129032258069</v>
+      </c>
+      <c r="J13">
         <v>1</v>
+      </c>
+      <c r="K13" s="1">
+        <f t="shared" si="3"/>
+        <v>4.166666666666667</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="D14">
+        <f>SUM(D2:D13)</f>
+        <v>39</v>
+      </c>
+      <c r="F14">
+        <f>SUM(F2:F13)</f>
+        <v>41</v>
+      </c>
+      <c r="H14">
+        <f>SUM(H2:H13)</f>
+        <v>31</v>
+      </c>
+      <c r="J14">
+        <f>SUM(J2:J13)</f>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1475,7 +1715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>

</xml_diff>